<commit_message>
ouf logique ecriture grille
</commit_message>
<xml_diff>
--- a/matrice_temps/horaire_A.xlsx
+++ b/matrice_temps/horaire_A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Equipes</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>2022-04-03</t>
+  </si>
+  <si>
+    <t>Modèle repartition concentre</t>
   </si>
 </sst>
 </file>
@@ -474,149 +477,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="10" width="15.7109375" customWidth="1"/>
+    <col min="1" max="10" width="15.7109375" customWidth="1"/>
     <col min="3" max="10" width="15.7109375" customWidth="1"/>
     <col min="4" max="10" width="15.7109375" customWidth="1"/>
     <col min="5" max="10" width="15.7109375" customWidth="1"/>
     <col min="6" max="10" width="15.7109375" customWidth="1"/>
     <col min="7" max="10" width="15.7109375" customWidth="1"/>
     <col min="8" max="10" width="15.7109375" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
+    <row r="11" spans="1:9">
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>34</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>